<commit_message>
Update to v 2022.3.8f1
</commit_message>
<xml_diff>
--- a/Bum's Away/Assets/_Documents/Downloads credits.xlsx
+++ b/Bum's Away/Assets/_Documents/Downloads credits.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>"Male and female body base mesh free to download" (https://skfb.ly/6QYp6) by Mr.Toadstool is licensed under Creative Commons Attribution (http://creativecommons.org/licenses/by/4.0/).</t>
   </si>
@@ -55,6 +55,24 @@
   </si>
   <si>
     <t>Fender stratocaster (https://skfb.ly/6Z8pF) by MANUGR is licensed under Creative Commons Attribution (http://creativecommons.org/licenses/by/4.0/).</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/3d-models/pubg-style-female-bus-driver-suit-free-2c3cb29c6cb44084bfe965d6fa887b21</t>
+  </si>
+  <si>
+    <t>Nathan</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/3d-models/nathan-animated-003-walking-3d-man-143a2b1ea5eb4385ae90a73657aca3bc</t>
+  </si>
+  <si>
+    <t>RenderPeople</t>
+  </si>
+  <si>
+    <t>Final Render Animation Studio</t>
   </si>
 </sst>
 </file>
@@ -498,16 +516,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3"/>
+  <dimension ref="A4:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="102.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="C11" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>